<commit_message>
Add and update address form validation tests
Added new Cypress tests for address form validation with special characters and updated test case numbering for consistency. Introduced a new custom command 'checkTextShouldBeEmptyOfAddressForm' to verify empty input fields by placeholder. Also removed an unused Excel file from the downloads directory.
</commit_message>
<xml_diff>
--- a/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
+++ b/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="269">
   <si>
     <t>ID</t>
   </si>
@@ -300,6 +300,35 @@
     <t>TC17</t>
   </si>
   <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập country là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập country là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: @@#$%#(*$@
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không nhập được kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập name</t>
   </si>
   <si>
@@ -322,7 +351,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a name."</t>
   </si>
   <si>
-    <t>TC18</t>
+    <t>TC19</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập mobile number</t>
@@ -347,7 +376,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a mobile number."</t>
   </si>
   <si>
-    <t>TC19</t>
+    <t>TC20</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number quá ngắn</t>
@@ -373,7 +402,7 @@
     <t>Hiển thị thông báo cảnh báo :   "Mobile number must match {{range}} format."</t>
   </si>
   <si>
-    <t>TC20</t>
+    <t>TC21</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number đúng tối thiểu</t>
@@ -399,13 +428,17 @@
     <t>Hợp lệ</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>M, H</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">ỗi xác thực sai khiến người dùng </t>
     </r>
     <r>
@@ -473,7 +506,7 @@
     </r>
   </si>
   <si>
-    <t>TC21</t>
+    <t>TC22</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number trung bình</t>
@@ -496,7 +529,7 @@
 State: Thanh Tri</t>
   </si>
   <si>
-    <t>TC22</t>
+    <t>TC23</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number cận tối đa</t>
@@ -519,7 +552,7 @@
 State: Thanh Tri</t>
   </si>
   <si>
-    <t>TC23</t>
+    <t>TC24</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number đúng tối đa</t>
@@ -532,7 +565,7 @@
 4. Nhập đầy đủ thông tin và nhập độ dài mobile number đúng tối đa</t>
   </si>
   <si>
-    <t>TC24</t>
+    <t>TC25</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number quá dài</t>
@@ -555,7 +588,7 @@
 State: Thanh Tri</t>
   </si>
   <si>
-    <t>TC25</t>
+    <t>TC26</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự . ở cuối</t>
@@ -584,6 +617,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Cần sửa trong chu kỳ kế tiếp để tránh </t>
     </r>
     <r>
@@ -609,7 +649,7 @@
     </r>
   </si>
   <si>
-    <t>TC26</t>
+    <t>TC27</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number chứa các kí tự chữ</t>
@@ -632,7 +672,7 @@
 State: Thanh Tri</t>
   </si>
   <si>
-    <t>TC27</t>
+    <t>TC28</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự + ở đầu</t>
@@ -661,7 +701,7 @@
     <t>L</t>
   </si>
   <si>
-    <t>TC28</t>
+    <t>TC29</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập zip code</t>
@@ -685,7 +725,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a Zip code."</t>
   </si>
   <si>
-    <t>TC29</t>
+    <t>TC30</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự đặc biệt</t>
@@ -715,6 +755,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Đây là lỗi </t>
     </r>
     <r>
@@ -761,7 +808,33 @@
     </r>
   </si>
   <si>
-    <t>TC30</t>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự chữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và zip code với các kí tự </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: winter
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không chấp nhận kí tự chữ</t>
+  </si>
+  <si>
+    <t>TC32</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập address</t>
@@ -786,7 +859,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide an address."</t>
   </si>
   <si>
-    <t>TC31</t>
+    <t>TC33</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &lt; 160</t>
@@ -802,7 +875,7 @@
     <t>Không hiện cảnh báo</t>
   </si>
   <si>
-    <t>TC32</t>
+    <t>TC34</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &gt; 160</t>
@@ -828,7 +901,7 @@
     <t>Không nhập được thêm nếu độ dài hơn 160</t>
   </si>
   <si>
-    <t>TC33</t>
+    <t>TC35</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập city</t>
@@ -852,7 +925,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a city."</t>
   </si>
   <si>
-    <t>TC34</t>
+    <t>TC36</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập country là khoảng trắng</t>
@@ -874,7 +947,7 @@
 City: Ha Noi</t>
   </si>
   <si>
-    <t>TC35</t>
+    <t>TC37</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập name là khoảng trắng</t>
@@ -896,7 +969,7 @@
 City: Ha Noi</t>
   </si>
   <si>
-    <t>TC36</t>
+    <t>TC38</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zipcode là khoảng trắng</t>
@@ -921,7 +994,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a zipcode."</t>
   </si>
   <si>
-    <t>TC37</t>
+    <t>TC39</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập address là khoảng trắng</t>
@@ -943,7 +1016,7 @@
 City: Ha Noi</t>
   </si>
   <si>
-    <t>TC38</t>
+    <t>TC40</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập city là khoảng trắng</t>
@@ -965,7 +1038,52 @@
 City: </t>
   </si>
   <si>
-    <t>TC39</t>
+    <t>TC41</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập city là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập city là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: @@#!</t>
+  </si>
+  <si>
+    <t>TC42</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập state là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập state là kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: @@#!</t>
+  </si>
+  <si>
+    <t>TC43</t>
   </si>
   <si>
     <t>Kiểm thử phương thức giao hàng khi mua hàng</t>
@@ -978,7 +1096,7 @@
 4. Chọn phương thức giao hàng</t>
   </si>
   <si>
-    <t>TC40</t>
+    <t>TC44</t>
   </si>
   <si>
     <t>Kiểm thử phương thức thanh toán khi mua hàng</t>
@@ -992,7 +1110,7 @@
 5. Chọn phương thức thanh toán</t>
   </si>
   <si>
-    <t>TC41</t>
+    <t>TC45</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập đầy đủ thông tin</t>
@@ -1016,7 +1134,7 @@
     <t>Hiện thẻ vừa thêm</t>
   </si>
   <si>
-    <t>TC42</t>
+    <t>TC46</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Name</t>
@@ -1037,7 +1155,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC43</t>
+    <t>TC47</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Card Number</t>
@@ -1060,7 +1178,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter your card number"</t>
   </si>
   <si>
-    <t>TC44</t>
+    <t>TC48</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Expiry Month</t>
@@ -1083,7 +1201,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter an Expiry Month"</t>
   </si>
   <si>
-    <t>TC45</t>
+    <t>TC49</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Expiry Year</t>
@@ -1101,7 +1219,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter an Expiry Year"</t>
   </si>
   <si>
-    <t>TC46</t>
+    <t>TC50</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập Name là khoảng trắng</t>
@@ -1122,7 +1240,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC47</t>
+    <t>TC51</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập Card Number là khoảng trắng</t>
@@ -1146,7 +1264,7 @@
     <t>Không nhập được khoảng trắng</t>
   </si>
   <si>
-    <t>TC48</t>
+    <t>TC52</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập độ dài Card Number &lt; 16</t>
@@ -1170,7 +1288,7 @@
     <t>Hiển thị thông báo cảnh báo :   "  Please enter a valid sixteen digit card number."</t>
   </si>
   <si>
-    <t>TC49</t>
+    <t>TC53</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập độ dài Card Number &gt; 16</t>
@@ -1191,7 +1309,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC50</t>
+    <t>TC54</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà coupon không hợp lệ</t>
@@ -1212,7 +1330,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Invalid coupon."</t>
   </si>
   <si>
-    <t>TC51</t>
+    <t>TC55</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà độ dài coupon &lt; 10</t>
@@ -1233,7 +1351,7 @@
     <t>Hiển thị thông báo cảnh báo :  " Coupon code must be 10 characters long."</t>
   </si>
   <si>
-    <t>TC52</t>
+    <t>TC56</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà độ dài coupon &gt; 10</t>
@@ -1251,7 +1369,7 @@
     <t>n(XRwh7ZQrr</t>
   </si>
   <si>
-    <t>TC53</t>
+    <t>TC57</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà coupon hợp lệ</t>
@@ -1273,7 +1391,7 @@
     <t>Hiển thị thông báo :   "Your discount of 30% will be applied during checkout."</t>
   </si>
   <si>
-    <t>TC54</t>
+    <t>TC58</t>
   </si>
   <si>
     <t>Kiểm thử thanh toán thành công khi mua hàng</t>
@@ -1291,7 +1409,7 @@
     <t>Hiển thị thông báo :   "Thank you for your purchase!"</t>
   </si>
   <si>
-    <t>TC55</t>
+    <t>TC59</t>
   </si>
   <si>
     <t>Kiểm thử thanh toán thành công khi mua hàng với mã giảm giá hợp lệ</t>
@@ -2486,10 +2604,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -2829,7 +2947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" ht="131.25" spans="1:6">
+    <row r="19" ht="150" spans="1:6">
       <c r="A19" s="9" t="s">
         <v>71</v>
       </c>
@@ -2845,111 +2963,111 @@
       <c r="E19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>11</v>
+      <c r="F19" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="20" ht="131.25" spans="1:6">
       <c r="A20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" ht="131.25" spans="1:6">
+      <c r="A21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" ht="150" spans="1:6">
+      <c r="A22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" ht="150" spans="1:8">
+      <c r="A23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" ht="150" spans="1:6">
-      <c r="A21" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" ht="300" spans="1:8">
-      <c r="A22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" ht="150" spans="1:6">
-      <c r="A23" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="G23" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>11</v>
+      <c r="H23" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="24" ht="150" spans="1:6">
       <c r="A24" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>11</v>
@@ -2957,19 +3075,19 @@
     </row>
     <row r="25" ht="150" spans="1:6">
       <c r="A25" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>11</v>
@@ -2977,117 +3095,117 @@
     </row>
     <row r="26" ht="150" spans="1:6">
       <c r="A26" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" ht="131.25" spans="1:8">
+    <row r="27" ht="150" spans="1:6">
       <c r="A27" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="E27" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="F27" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" ht="131.25" spans="1:8">
+      <c r="A28" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H27" t="s">
+      <c r="B28" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" ht="150" spans="1:7">
-      <c r="A28" s="9" t="s">
+      <c r="C28" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="F28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>114</v>
+      <c r="H28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" ht="150" spans="1:7">
       <c r="A29" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G29" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" ht="150" spans="1:7">
+      <c r="A30" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" ht="112.5" spans="1:6">
-      <c r="A30" s="9" t="s">
+      <c r="B30" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" ht="150" spans="1:8">
+    </row>
+    <row r="31" ht="112.5" spans="1:6">
       <c r="A31" s="9" t="s">
         <v>131</v>
       </c>
@@ -3103,34 +3221,34 @@
       <c r="E31" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" ht="150" spans="1:8">
+      <c r="A32" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H31" t="s">
+      <c r="B32" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" ht="131.25" spans="1:6">
-      <c r="A32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="F32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="H32" t="s">
         <v>142</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="33" ht="150" spans="1:6">
@@ -3144,47 +3262,47 @@
         <v>145</v>
       </c>
       <c r="D33" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" ht="131.25" spans="1:6">
+      <c r="A34" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" ht="150" spans="1:6">
+      <c r="A35" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" ht="206.25" spans="1:6">
-      <c r="A34" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" ht="112.5" spans="1:6">
-      <c r="A35" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>155</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>156</v>
@@ -3193,7 +3311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" ht="131.25" spans="1:7">
+    <row r="36" ht="206.25" spans="1:6">
       <c r="A36" s="9" t="s">
         <v>157</v>
       </c>
@@ -3207,218 +3325,218 @@
         <v>160</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" ht="131.25" spans="1:7">
+        <v>161</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" ht="112.5" spans="1:6">
       <c r="A37" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>114</v>
+        <v>166</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" ht="131.25" spans="1:7">
       <c r="A38" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>169</v>
+        <v>70</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" ht="131.25" spans="1:7">
       <c r="A39" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" ht="131.25" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" ht="93.75" spans="1:6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" ht="131.25" spans="1:7">
       <c r="A41" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D41" s="10"/>
+        <v>182</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>183</v>
+      </c>
       <c r="E41" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" ht="112.5" spans="1:6">
+        <v>152</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" ht="131.25" spans="1:7">
       <c r="A42" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D42" s="10"/>
+        <v>186</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>187</v>
+      </c>
       <c r="E42" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>11</v>
+        <v>166</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="43" ht="131.25" spans="1:6">
       <c r="A43" s="9" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" ht="131.25" spans="1:6">
+        <v>75</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" ht="150" spans="1:6">
       <c r="A44" s="9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" ht="131.25" spans="1:6">
+      <c r="F44" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" ht="93.75" spans="1:6">
       <c r="A45" s="9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>196</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="D45" s="10"/>
       <c r="E45" s="10" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" ht="131.25" spans="1:6">
+    <row r="46" ht="112.5" spans="1:6">
       <c r="A46" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D46" s="10" t="s">
         <v>201</v>
       </c>
+      <c r="D46" s="10"/>
       <c r="E46" s="10" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>11</v>
@@ -3426,16 +3544,16 @@
     </row>
     <row r="47" ht="131.25" spans="1:6">
       <c r="A47" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="D47" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>187</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>206</v>
@@ -3444,7 +3562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" ht="131.25" spans="1:7">
+    <row r="48" ht="131.25" spans="1:6">
       <c r="A48" s="9" t="s">
         <v>207</v>
       </c>
@@ -3458,16 +3576,13 @@
         <v>210</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" ht="150" spans="1:6">
+        <v>81</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" ht="131.25" spans="1:6">
       <c r="A49" s="9" t="s">
         <v>211</v>
       </c>
@@ -3518,16 +3633,16 @@
         <v>223</v>
       </c>
       <c r="D51" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E51" s="10" t="s">
-        <v>220</v>
-      </c>
       <c r="F51" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" ht="131.25" spans="1:6">
+    <row r="52" ht="131.25" spans="1:7">
       <c r="A52" s="9" t="s">
         <v>225</v>
       </c>
@@ -3541,27 +3656,30 @@
         <v>228</v>
       </c>
       <c r="E52" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" ht="150" spans="1:6">
+      <c r="A53" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" ht="131.25" spans="1:6">
-      <c r="A53" s="9" t="s">
+      <c r="B53" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="E53" s="10" t="s">
         <v>233</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>234</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>11</v>
@@ -3569,25 +3687,25 @@
     </row>
     <row r="54" ht="131.25" spans="1:6">
       <c r="A54" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="C54" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="E54" s="10" t="s">
-        <v>234</v>
-      </c>
       <c r="F54" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" ht="150" spans="1:6">
+    <row r="55" ht="131.25" spans="1:6">
       <c r="A55" s="9" t="s">
         <v>239</v>
       </c>
@@ -3601,7 +3719,7 @@
         <v>242</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>11</v>
@@ -3609,15 +3727,17 @@
     </row>
     <row r="56" ht="131.25" spans="1:6">
       <c r="A56" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="D56" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="D56" s="10"/>
       <c r="E56" s="10" t="s">
         <v>247</v>
       </c>
@@ -3625,7 +3745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" ht="150" spans="1:6">
+    <row r="57" ht="131.25" spans="1:6">
       <c r="A57" s="9" t="s">
         <v>248</v>
       </c>
@@ -3636,12 +3756,90 @@
         <v>250</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F57" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" ht="131.25" spans="1:6">
+      <c r="A58" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" ht="150" spans="1:6">
+      <c r="A59" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" ht="131.25" spans="1:6">
+      <c r="A60" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" ht="150" spans="1:6">
+      <c r="A61" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F61" s="11" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add user authentication middleware
Introduced a new middleware to handle user authentication for protected routes. This ensures that only authenticated users can access certain endpoints.
</commit_message>
<xml_diff>
--- a/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
+++ b/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18285"/>
+    <workbookView windowWidth="19200" windowHeight="18300"/>
   </bookViews>
   <sheets>
     <sheet name="Search Test Cases" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="267">
   <si>
     <t>ID</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Kiểm thử chức năng mua hàng</t>
   </si>
   <si>
-    <t>TC01</t>
+    <t>DH_01</t>
   </si>
   <si>
     <t>Kiểm thử thêm 1 sản phẩm vào giỏ hàng ở trang chủ</t>
@@ -66,7 +66,7 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>TC02</t>
+    <t>DH_02</t>
   </si>
   <si>
     <t>Kiểm thử thêm 1 sản phẩm nhiều lần vào giỏ hàng ở trang chủ</t>
@@ -79,7 +79,7 @@
     <t>Thấy sản phẩm vừa thêm ở giỏ hàng và đúng số lượng đã thêm</t>
   </si>
   <si>
-    <t>TC03</t>
+    <t>DH_03</t>
   </si>
   <si>
     <t>Kiểm thử thêm nhiều sản phẩm khác nhau vào giỏ hàng ở trang chủ</t>
@@ -92,7 +92,7 @@
     <t>Thấy các sản phẩm vừa thêm</t>
   </si>
   <si>
-    <t>TC04</t>
+    <t>DH_04</t>
   </si>
   <si>
     <t>Kiểm thử tăng số lượng sản phẩm trong giỏ hàng</t>
@@ -106,7 +106,7 @@
     <t>Thấy số lượng sản phẩm tăng</t>
   </si>
   <si>
-    <t>TC05</t>
+    <t>DH_05</t>
   </si>
   <si>
     <t>Kiểm thử giảm số lượng sản phẩm trong giỏ hàng</t>
@@ -120,7 +120,7 @@
     <t>Thấy số lượng sản phẩm giảm</t>
   </si>
   <si>
-    <t>TC06</t>
+    <t>DH_06</t>
   </si>
   <si>
     <t>Kiểm thử xóa một sản phẩm sản phẩm trong giỏ hàng</t>
@@ -134,7 +134,7 @@
     <t>Không thấy sản phẩm vừa xóa trong giỏ hàng</t>
   </si>
   <si>
-    <t>TC07</t>
+    <t>DH_07</t>
   </si>
   <si>
     <t>Kiểm thử xóa tất cả sản phẩm trong giỏ hàng</t>
@@ -148,7 +148,7 @@
     <t>Không thấy sản phẩm nào trong giỏ hàng</t>
   </si>
   <si>
-    <t>TC08</t>
+    <t>DH_08</t>
   </si>
   <si>
     <t>Kiểm thử cập nhật tổng tiền sau khi tăng số lượng sản phẩm</t>
@@ -157,7 +157,7 @@
     <t>Thấy tổng tiền tăng đúng</t>
   </si>
   <si>
-    <t>TC09</t>
+    <t>DH_09</t>
   </si>
   <si>
     <t>Kiểm thử cập nhật tổng tiền sau khi giảm số lượng sản phẩm</t>
@@ -171,7 +171,7 @@
     <t>Thấy tổng tiền giảm đúng</t>
   </si>
   <si>
-    <t>TC10</t>
+    <t>DH_10</t>
   </si>
   <si>
     <t>Kiểm thử cập nhật tổng tiền sau khi xóa một sản phẩm</t>
@@ -182,7 +182,7 @@
 3. Nhấn biểu tượng thùng rác </t>
   </si>
   <si>
-    <t>TC11</t>
+    <t>DH_11</t>
   </si>
   <si>
     <t>Kiểm thử cập nhật tổng tiền sau khi xóa tất cả sản phẩm</t>
@@ -191,7 +191,7 @@
     <t>Thấy tổng tiền bằng 0</t>
   </si>
   <si>
-    <t>TC12</t>
+    <t>DH_12</t>
   </si>
   <si>
     <t>Kiểm thử chọn địa chỉ khi mua hàng</t>
@@ -206,7 +206,7 @@
     <t>Nút continue được bật</t>
   </si>
   <si>
-    <t>TC13</t>
+    <t>DH_13</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không điền thông tin nào</t>
@@ -222,7 +222,7 @@
     <t>Không thể ấn nút Submit</t>
   </si>
   <si>
-    <t>TC14</t>
+    <t>DH_14</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mà không nhập state</t>
@@ -248,7 +248,7 @@
     <t>Thêm thành công địa chỉ mới</t>
   </si>
   <si>
-    <t>TC15</t>
+    <t>DH_15</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập đầy đủ thông tin</t>
@@ -272,7 +272,7 @@
 State: Thanh Tri</t>
   </si>
   <si>
-    <t>TC16</t>
+    <t>DH_16</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập country</t>
@@ -297,7 +297,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a country."</t>
   </si>
   <si>
-    <t>TC17</t>
+    <t>DH_17</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập country là kí tự đặc biệt</t>
@@ -326,7 +326,10 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>TC18</t>
+    <t>L</t>
+  </si>
+  <si>
+    <t>DH_18</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập name</t>
@@ -351,7 +354,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a name."</t>
   </si>
   <si>
-    <t>TC19</t>
+    <t>DH_19</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập mobile number</t>
@@ -376,7 +379,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a mobile number."</t>
   </si>
   <si>
-    <t>TC20</t>
+    <t>DH_20</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number quá ngắn</t>
@@ -402,7 +405,7 @@
     <t>Hiển thị thông báo cảnh báo :   "Mobile number must match {{range}} format."</t>
   </si>
   <si>
-    <t>TC21</t>
+    <t>DH_21</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number đúng tối thiểu</t>
@@ -428,7 +431,380 @@
     <t>Hợp lệ</t>
   </si>
   <si>
-    <t>M, H</t>
+    <t>DH_22</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number trung bình</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập độ dài mobile number trung bình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 08673336
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>DH_23</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number cận tối đa</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập độ dài mobile number cận tối đa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 086733369
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>DH_24</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number đúng tối đa</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập độ dài mobile number đúng tối đa</t>
+  </si>
+  <si>
+    <t>DH_25</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number quá dài</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập độ dài mobile number quá dài</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 086733369777
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>DH_26</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự . ở cuối</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập mobile number với ký tự . ở cuối</t>
+  </si>
+  <si>
+    <t>Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 08673333.69
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Hiện thi thông báo lỗi</t>
+  </si>
+  <si>
+    <t>DH_27</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number chứa các kí tự chữ</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập mobile number chứa các ký tự chữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 777e7
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>DH_28</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự + ở đầu</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập mobile number với ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: +11111111 
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không nhập được ký tự +</t>
+  </si>
+  <si>
+    <t>DH_29</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập zip code</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và không nhập zip code</t>
+  </si>
+  <si>
+    <t>Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo cảnh báo :   " Please provide a Zip code."</t>
+  </si>
+  <si>
+    <t>DH_30</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và zip code với các kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: @@#!
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không chấp nhận kí tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Vì nếu hệ thống không cho nhập ZIP chứa ký tự đặc biệt nhưng không có cảnh báo hoặc xử lý không rõ ràng, thì đây là lỗi nhỏ về trải nghiệm người dùng.</t>
+  </si>
+  <si>
+    <t>DH_31</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự chữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và zip code với các kí tự </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: winter
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không chấp nhận kí tự chữ</t>
+  </si>
+  <si>
+    <t>Vì nếu hệ thống không cho nhập ZIP chứa ký tự chữ nhưng không có cảnh báo hoặc xử lý không rõ ràng, thì đây là lỗi nhỏ về trải nghiệm người dùng.</t>
+  </si>
+  <si>
+    <t>DH_32</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập address</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và không nhập address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo cảnh báo :   " Please provide an address."</t>
+  </si>
+  <si>
+    <t>DH_33</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &lt; 160</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và độ dài address &lt; 160</t>
+  </si>
+  <si>
+    <t>Không hiện cảnh báo</t>
+  </si>
+  <si>
+    <t>DH_34</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &gt; 160</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và độ dài address &gt; 160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: orem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an 
+City: Ha Noi
+State: Thanh Tri</t>
+  </si>
+  <si>
+    <t>Không nhập được thêm nếu độ dài hơn 160</t>
+  </si>
+  <si>
+    <t>DH_35</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập city</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và không nhập city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo cảnh báo :   " Please provide a city."</t>
+  </si>
+  <si>
+    <t>DH_36</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập country là khoảng trắng</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập country là khoảng trắng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: 
+Name: Phan Hong Quan
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi</t>
+  </si>
+  <si>
+    <t>Trường Country thường dùng để tính phí ship, thuế, kiểm tra hợp lệ đơn hàng, nên nếu để trống mà không cảnh báo có thể gây hậu quả về sau.</t>
+  </si>
+  <si>
+    <t>DH_37</t>
+  </si>
+  <si>
+    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập name là khoảng trắng</t>
+  </si>
+  <si>
+    <t>1. Thêm sản phẩm vào giỏ hàng 
+2. Mở giỏ hàng
+2. Nhấn checkout để sang trang chọn địa chỉ
+3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
+4. Nhập đầy đủ thông tin và nhập name là khoảng trắng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Viet Nam
+Name: 
+Mobile Number: 0867333697
+Zip Code: 10000
+Address: Tan Trieu, Thanh Tri, Ha Noi
+City: Ha Noi</t>
   </si>
   <si>
     <r>
@@ -439,7 +815,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">ỗi xác thực sai khiến người dùng </t>
+      <t xml:space="preserve">Trường Country </t>
     </r>
     <r>
       <rPr>
@@ -450,7 +826,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>không thể mua hàng</t>
+      <t>thường dùng để tính phí ship, thuế, kiểm tra hợp lệ đơn hàng</t>
     </r>
     <r>
       <rPr>
@@ -460,516 +836,11 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, ảnh hưởng </t>
+      <t>, nên nếu để trống mà không cảnh báo có thể gây hậu quả về sau.</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>trực tiếp đến chức năng kinh doanh chính</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> → </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>phải được xử lý ngay lập tức</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number trung bình</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập độ dài mobile number trung bình</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 08673336
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number cận tối đa</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập độ dài mobile number cận tối đa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 086733369
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number đúng tối đa</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập độ dài mobile number đúng tối đa</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài mobile number quá dài</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập độ dài mobile number quá dài</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 086733369777
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>TC26</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự . ở cuối</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập mobile number với ký tự . ở cuối</t>
-  </si>
-  <si>
-    <t>Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 08673333.69
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Hiện thi thông báo lỗi</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Cần sửa trong chu kỳ kế tiếp để tránh </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nhập sai dữ liệu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> gây hậu quả về sau.</t>
-    </r>
-  </si>
-  <si>
-    <t>TC27</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number chứa các kí tự chữ</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập mobile number chứa các ký tự chữ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 777e7
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>TC28</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập mobile number với ký tự + ở đầu</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập mobile number với ký tự đặc biệt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: +11111111 
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Không nhập được ký tự +</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>TC29</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập zip code</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và không nhập zip code</t>
-  </si>
-  <si>
-    <t>Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Hiển thị thông báo cảnh báo :   " Please provide a Zip code."</t>
-  </si>
-  <si>
-    <t>TC30</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự đặc biệt</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và zip code với các kí tự đặc biệt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: @@#!
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Không chấp nhận kí tự đặc biệt</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Đây là lỗi </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>đầu vào dữ liệu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> có thể ảnh hưởng đến quá trình xử lý đơn hàng hoặc hậu cần, nên </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cần sửa trong chu kỳ phát triển kế tiếp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> để đảm bảo độ tin cậy và an toàn của hệ thống.</t>
-    </r>
-  </si>
-  <si>
-    <t>TC31</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zip code với các kí tự chữ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và zip code với các kí tự </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: winter
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Không chấp nhận kí tự chữ</t>
-  </si>
-  <si>
-    <t>TC32</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập address</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và không nhập address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: 10000
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Hiển thị thông báo cảnh báo :   " Please provide an address."</t>
-  </si>
-  <si>
-    <t>TC33</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &lt; 160</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và độ dài address &lt; 160</t>
-  </si>
-  <si>
-    <t>Không hiện cảnh báo</t>
-  </si>
-  <si>
-    <t>TC34</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập độ dài address &gt; 160</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và độ dài address &gt; 160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: 10000
-Address: orem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an 
-City: Ha Noi
-State: Thanh Tri</t>
-  </si>
-  <si>
-    <t>Không nhập được thêm nếu độ dài hơn 160</t>
-  </si>
-  <si>
-    <t>TC35</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà không nhập city</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và không nhập city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi</t>
-  </si>
-  <si>
-    <t>Hiển thị thông báo cảnh báo :   " Please provide a city."</t>
-  </si>
-  <si>
-    <t>TC36</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập country là khoảng trắng</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập country là khoảng trắng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: 
-Name: Phan Hong Quan
-Mobile Number: 0867333697
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi</t>
-  </si>
-  <si>
-    <t>TC37</t>
-  </si>
-  <si>
-    <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập name là khoảng trắng</t>
-  </si>
-  <si>
-    <t>1. Thêm sản phẩm vào giỏ hàng 
-2. Mở giỏ hàng
-2. Nhấn checkout để sang trang chọn địa chỉ
-3. Nhấn Add New Address để sang trang điền thông tin địa chỉ 
-4. Nhập đầy đủ thông tin và nhập name là khoảng trắng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Country: Viet Nam
-Name: 
-Mobile Number: 0867333697
-Zip Code: 10000
-Address: Tan Trieu, Thanh Tri, Ha Noi
-City: Ha Noi</t>
-  </si>
-  <si>
-    <t>TC38</t>
+  </si>
+  <si>
+    <t>DH_38</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập zipcode là khoảng trắng</t>
@@ -994,7 +865,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please provide a zipcode."</t>
   </si>
   <si>
-    <t>TC39</t>
+    <t>DH_39</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập address là khoảng trắng</t>
@@ -1016,7 +887,7 @@
 City: Ha Noi</t>
   </si>
   <si>
-    <t>TC40</t>
+    <t>DH_40</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập city là khoảng trắng</t>
@@ -1038,7 +909,7 @@
 City: </t>
   </si>
   <si>
-    <t>TC41</t>
+    <t>DH_41</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập city là kí tự đặc biệt</t>
@@ -1060,7 +931,7 @@
 City: @@#!</t>
   </si>
   <si>
-    <t>TC42</t>
+    <t>DH_42</t>
   </si>
   <si>
     <t>Kiểm thử nhập địa chỉ mua hàng mới mà nhập state là kí tự đặc biệt</t>
@@ -1083,7 +954,7 @@
 State: @@#!</t>
   </si>
   <si>
-    <t>TC43</t>
+    <t>DH_43</t>
   </si>
   <si>
     <t>Kiểm thử phương thức giao hàng khi mua hàng</t>
@@ -1096,7 +967,7 @@
 4. Chọn phương thức giao hàng</t>
   </si>
   <si>
-    <t>TC44</t>
+    <t>DH_44</t>
   </si>
   <si>
     <t>Kiểm thử phương thức thanh toán khi mua hàng</t>
@@ -1110,7 +981,7 @@
 5. Chọn phương thức thanh toán</t>
   </si>
   <si>
-    <t>TC45</t>
+    <t>DH_45</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập đầy đủ thông tin</t>
@@ -1134,7 +1005,7 @@
     <t>Hiện thẻ vừa thêm</t>
   </si>
   <si>
-    <t>TC46</t>
+    <t>DH_46</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Name</t>
@@ -1155,7 +1026,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC47</t>
+    <t>DH_47</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Card Number</t>
@@ -1178,7 +1049,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter your card number"</t>
   </si>
   <si>
-    <t>TC48</t>
+    <t>DH_48</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Expiry Month</t>
@@ -1201,7 +1072,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter an Expiry Month"</t>
   </si>
   <si>
-    <t>TC49</t>
+    <t>DH_49</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà không nhập Expiry Year</t>
@@ -1219,7 +1090,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Please enter an Expiry Year"</t>
   </si>
   <si>
-    <t>TC50</t>
+    <t>DH_50</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập Name là khoảng trắng</t>
@@ -1240,7 +1111,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC51</t>
+    <t>DH_51</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập Card Number là khoảng trắng</t>
@@ -1264,7 +1135,7 @@
     <t>Không nhập được khoảng trắng</t>
   </si>
   <si>
-    <t>TC52</t>
+    <t>DH_52</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập độ dài Card Number &lt; 16</t>
@@ -1288,7 +1159,7 @@
     <t>Hiển thị thông báo cảnh báo :   "  Please enter a valid sixteen digit card number."</t>
   </si>
   <si>
-    <t>TC53</t>
+    <t>DH_53</t>
   </si>
   <si>
     <t>Kiểm thử thêm thẻ thanh toán mà nhập độ dài Card Number &gt; 16</t>
@@ -1309,7 +1180,7 @@
 Expiry Year: 2099</t>
   </si>
   <si>
-    <t>TC54</t>
+    <t>DH_54</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà coupon không hợp lệ</t>
@@ -1330,7 +1201,7 @@
     <t>Hiển thị thông báo cảnh báo :   " Invalid coupon."</t>
   </si>
   <si>
-    <t>TC55</t>
+    <t>DH_55</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà độ dài coupon &lt; 10</t>
@@ -1351,7 +1222,7 @@
     <t>Hiển thị thông báo cảnh báo :  " Coupon code must be 10 characters long."</t>
   </si>
   <si>
-    <t>TC56</t>
+    <t>DH_56</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà độ dài coupon &gt; 10</t>
@@ -1369,7 +1240,7 @@
     <t>n(XRwh7ZQrr</t>
   </si>
   <si>
-    <t>TC57</t>
+    <t>DH_57</t>
   </si>
   <si>
     <t>Kiểm thử nhập coupon khi mua hàng mà coupon hợp lệ</t>
@@ -1391,7 +1262,7 @@
     <t>Hiển thị thông báo :   "Your discount of 30% will be applied during checkout."</t>
   </si>
   <si>
-    <t>TC58</t>
+    <t>DH_58</t>
   </si>
   <si>
     <t>Kiểm thử thanh toán thành công khi mua hàng</t>
@@ -1409,7 +1280,7 @@
     <t>Hiển thị thông báo :   "Thank you for your purchase!"</t>
   </si>
   <si>
-    <t>TC59</t>
+    <t>DH_59</t>
   </si>
   <si>
     <t>Kiểm thử thanh toán thành công khi mua hàng với mã giảm giá hợp lệ</t>
@@ -2208,7 +2079,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2248,8 +2119,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2606,8 +2487,8 @@
   <sheetPr/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -2947,7 +2828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" ht="150" spans="1:6">
+    <row r="19" ht="150" spans="1:7">
       <c r="A19" s="9" t="s">
         <v>71</v>
       </c>
@@ -2966,22 +2847,25 @@
       <c r="F19" s="13" t="s">
         <v>76</v>
       </c>
+      <c r="G19" s="14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="20" ht="131.25" spans="1:6">
       <c r="A20" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>11</v>
@@ -2989,19 +2873,19 @@
     </row>
     <row r="21" ht="131.25" spans="1:6">
       <c r="A21" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>11</v>
@@ -3009,19 +2893,19 @@
     </row>
     <row r="22" ht="150" spans="1:6">
       <c r="A22" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>11</v>
@@ -3029,45 +2913,43 @@
     </row>
     <row r="23" ht="150" spans="1:8">
       <c r="A23" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>76</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>98</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" ht="150" spans="1:6">
       <c r="A24" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="E24" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>11</v>
@@ -3075,19 +2957,19 @@
     </row>
     <row r="25" ht="150" spans="1:6">
       <c r="A25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="E25" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>11</v>
@@ -3095,19 +2977,19 @@
     </row>
     <row r="26" ht="150" spans="1:6">
       <c r="A26" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>11</v>
@@ -3115,19 +2997,19 @@
     </row>
     <row r="27" ht="150" spans="1:6">
       <c r="A27" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>113</v>
-      </c>
       <c r="E27" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>11</v>
@@ -3135,91 +3017,89 @@
     </row>
     <row r="28" ht="131.25" spans="1:8">
       <c r="A28" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>76</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" t="s">
-        <v>120</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" ht="150" spans="1:7">
       <c r="A29" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="E29" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>76</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" ht="150" spans="1:7">
       <c r="A30" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="E30" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>129</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>76</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" ht="112.5" spans="1:6">
       <c r="A31" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>11</v>
@@ -3227,65 +3107,71 @@
     </row>
     <row r="32" ht="150" spans="1:8">
       <c r="A32" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" ht="150" spans="1:8">
+      <c r="A33" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H32" t="s">
+      <c r="E33" s="10" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="33" ht="150" spans="1:6">
-      <c r="A33" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>76</v>
       </c>
+      <c r="G33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="34" ht="131.25" spans="1:6">
       <c r="A34" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>11</v>
@@ -3293,19 +3179,19 @@
     </row>
     <row r="35" ht="150" spans="1:6">
       <c r="A35" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>11</v>
@@ -3313,19 +3199,19 @@
     </row>
     <row r="36" ht="206.25" spans="1:6">
       <c r="A36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>11</v>
@@ -3333,36 +3219,36 @@
     </row>
     <row r="37" ht="112.5" spans="1:6">
       <c r="A37" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="F37" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" ht="141.75" spans="1:8">
+      <c r="A38" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" ht="131.25" spans="1:7">
-      <c r="A38" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>70</v>
@@ -3370,114 +3256,120 @@
       <c r="F38" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" ht="131.25" spans="1:7">
+      <c r="G38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" ht="135" spans="1:8">
       <c r="A39" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="E39" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>119</v>
+      <c r="G39" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="40" ht="131.25" spans="1:7">
       <c r="A40" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>119</v>
+      <c r="G40" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="41" ht="131.25" spans="1:7">
       <c r="A41" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>183</v>
-      </c>
       <c r="E41" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>119</v>
+      <c r="G41" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="42" ht="131.25" spans="1:7">
       <c r="A42" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>187</v>
-      </c>
       <c r="E42" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" ht="131.25" spans="1:6">
+      <c r="G42" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" ht="131.25" spans="1:7">
       <c r="A43" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>75</v>
@@ -3485,19 +3377,22 @@
       <c r="F43" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" ht="150" spans="1:6">
+      <c r="G43" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" ht="150" spans="1:7">
       <c r="A44" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>75</v>
@@ -3505,16 +3400,19 @@
       <c r="F44" s="13" t="s">
         <v>76</v>
       </c>
+      <c r="G44" s="14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="45" ht="93.75" spans="1:6">
       <c r="A45" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10" t="s">
@@ -3526,13 +3424,13 @@
     </row>
     <row r="46" ht="112.5" spans="1:6">
       <c r="A46" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10" t="s">
@@ -3544,19 +3442,19 @@
     </row>
     <row r="47" ht="131.25" spans="1:6">
       <c r="A47" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="D47" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>204</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>206</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>11</v>
@@ -3564,19 +3462,19 @@
     </row>
     <row r="48" ht="131.25" spans="1:6">
       <c r="A48" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="E48" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F48" s="11" t="s">
         <v>11</v>
@@ -3584,19 +3482,19 @@
     </row>
     <row r="49" ht="131.25" spans="1:6">
       <c r="A49" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="E49" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>215</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>11</v>
@@ -3604,19 +3502,19 @@
     </row>
     <row r="50" ht="131.25" spans="1:6">
       <c r="A50" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>11</v>
@@ -3624,19 +3522,19 @@
     </row>
     <row r="51" ht="131.25" spans="1:6">
       <c r="A51" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="D51" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>222</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>11</v>
@@ -3644,42 +3542,42 @@
     </row>
     <row r="52" ht="131.25" spans="1:7">
       <c r="A52" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>228</v>
-      </c>
       <c r="E52" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>119</v>
+      <c r="G52" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="53" ht="150" spans="1:6">
       <c r="A53" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="E53" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>233</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>11</v>
@@ -3687,19 +3585,19 @@
     </row>
     <row r="54" ht="131.25" spans="1:6">
       <c r="A54" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>11</v>
@@ -3707,19 +3605,19 @@
     </row>
     <row r="55" ht="131.25" spans="1:6">
       <c r="A55" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="D55" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>242</v>
-      </c>
       <c r="E55" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>11</v>
@@ -3727,19 +3625,19 @@
     </row>
     <row r="56" ht="131.25" spans="1:6">
       <c r="A56" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="D56" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="E56" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>247</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>11</v>
@@ -3747,19 +3645,19 @@
     </row>
     <row r="57" ht="131.25" spans="1:6">
       <c r="A57" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="D57" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>11</v>
@@ -3767,19 +3665,19 @@
     </row>
     <row r="58" ht="131.25" spans="1:6">
       <c r="A58" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="D58" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>256</v>
-      </c>
       <c r="E58" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>11</v>
@@ -3787,19 +3685,19 @@
     </row>
     <row r="59" ht="150" spans="1:6">
       <c r="A59" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="D59" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="E59" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>11</v>
@@ -3807,17 +3705,17 @@
     </row>
     <row r="60" ht="131.25" spans="1:6">
       <c r="A60" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>11</v>
@@ -3825,19 +3723,19 @@
     </row>
     <row r="61" ht="150" spans="1:6">
       <c r="A61" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="B61" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>268</v>
-      </c>
       <c r="D61" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Update test suite description for order functionality
Changed the test suite description from 'mua hàng' (purchase) to 'đặt hàng' (order) in juice_cart.cy.js to better reflect the tested functionality. Updated related Excel file with new test data or results.
</commit_message>
<xml_diff>
--- a/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
+++ b/OWASP_JUICE_SHOP_CART_FEATURES_CYPRESS_TESTING_FINAL (4).xlsx
@@ -50,7 +50,7 @@
     <t>Mức độ lỗi</t>
   </si>
   <si>
-    <t>Kiểm thử chức năng mua hàng</t>
+    <t>Kiểm thử chức năng đặt hàng</t>
   </si>
   <si>
     <t>DH_01</t>
@@ -2548,8 +2548,8 @@
   <sheetPr/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>

</xml_diff>